<commit_message>
added recovery of 072072D782D
</commit_message>
<xml_diff>
--- a/deployed_tags.xlsx
+++ b/deployed_tags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ssd980/gits/oxbow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA898B59-55B6-439A-B448-F888296352C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A8D44-7D5F-2445-BAFD-46F6E89B9554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21260" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="70">
   <si>
     <t>tag_id</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>1E554B19</t>
+  </si>
+  <si>
+    <t>2023-06-11 12:47</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1094,20 +1097,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="9" max="9" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="3"/>
+    <col min="9" max="9" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>55613319</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>44754</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>19611933</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>66667855</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>34616633</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>55616107</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>55526107</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
@@ -1762,8 +1765,11 @@
       <c r="H25" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="J25" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>68</v>
       </c>

</xml_diff>